<commit_message>
Get daily reddit data: Tue Aug 13 08:09:27 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C469"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2862 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1er20rx</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>First time using gel and some stones! How did I do?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1er20rx/first_time_using_gel_and_some_stones_how_did_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1er1zi6</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>The pebbles give it the special touch..</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsqvb0zpydid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1er1t29</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Which shape is best for appearance and durability?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er1t29</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1er1j65</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Good stick on tape?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er1j65</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1er1j29</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else have a nail tray? </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3k6f1r5tdid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1er1i0y</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>rewarding myself with some champagne cateye nails</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fx6nd7rsdid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1er1g7t</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">any good nail tech recommendations in LA? </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1er1g7t/any_good_nail_tech_recommendations_in_la/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1er159k</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>blue nail art😄</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djkh833oodid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1er12nb</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>my favorite nails set</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t93ufa9nndid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1er0hpd</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>3D floral frenchiezzz</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er0hpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1eqzx3f</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting square nails </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e00jbn7x9did1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1eqztrv</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic but cute </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsdh00dv8did1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1eqw4g2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail newbie </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqw4g2/nail_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1eqzggr</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>did these myself 🥰</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9immczu4did1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1eqyt1p</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails amazing work </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqyt1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1eqypqx</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a teal swirl moment </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sazl44r6xcid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1eqy3pu</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue advice </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqy3pu/glue_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1eqy0s8</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>literally just a girl</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqy0s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1eqxzum</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>What do you girls think? honestly 🩵🩵🩵</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqxzum</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1eqx62q</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My acrylic journey (swipe)</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqx62q</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1eqwf7a</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>I’m so proud of this set 🤭🐞❤️</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoqbe5c7ccid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1eqwb67</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>First set in months!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqwb67</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1eqw2bl</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">builder gel nail journey </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqw2bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1eqq8yz</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">online course recc </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqq8yz/online_course_recc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1equrcg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Liquid gel full set upkeep</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1equrcg/liquid_gel_full_set_upkeep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1eqvsuw</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">boxing with fake nails </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqvsuw/boxing_with_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1eqvtd1</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emergency nails </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqvtd1/emergency_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1eqvrjc</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shrek rave nails </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqvrjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1eqvr96</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>What nail shape looks better on me? Oval or Square?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqvr96</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1eqr8xw</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Can someone please explain to me what each of these nail drill bits are for? Trying to start doing my own nails instead of going to the salon and getting acrylics. Hoping to do press on nails. I got this from Amazon from the brand Yayabb but there is literally no instructions on what each one is for</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqr8xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1equ8op</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need help deciding on which shape is better! </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1equ8op</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1eqv986</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Issue with Gel Nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqv986/issue_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1eqv3xb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>I got dip powder nails done! 🖤</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbdw4fou0cid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1eqv2m0</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>red red red</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqv2m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1equwiu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>New set. Not sure how I feel about them</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrv8kjz5zbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1equqr0</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Korean/Japanese style nails in Cleveland, OH? </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1equqr0/koreanjapanese_style_nails_in_cleveland_oh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1equitk</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried Sistaco mineral nail powder </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1equitk</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1equdi1</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Cloudy Sky ☁️</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1equdi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1eqtyq8</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I haven’t perfected taking photos. </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqtyq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1eqtv12</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French with a wave, what do you think... Natural </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzts0napqbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1eqt1n8</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>new nudies :D</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqt1n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1eqsyot</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>stamping of mickey mouse</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wpus10ljbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1eqseon</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Ultra Frequent Gel Manicure with Peel Off Base</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqseon/ultra_frequent_gel_manicure_with_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1eqsb0r</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting square nails </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi3i1l9jebid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1eqs7sl</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squoval impress nails &gt; oval impress nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqs7sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1eqqzsa</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>C-hill out</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frl7kuql4bid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1eqna0v</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>My first gelx nails!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2xytxd6eaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1eqmr9w</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Posted this on my instagram and received a dm saying they were pretty to look at but not to wear. I’d really like opinions on this statement </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcmaxldgaaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1eqllkt</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>I just want to feel pretty again</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqllkt/i_just_want_to_feel_pretty_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1eqs1hx</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>I can't take my eyes off of them.</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nglh8ilcbid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1eqrjwx</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Prepped 🙌🏻</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqrjwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1eqr7jh</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Multicolored - but on toes - thoughts?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jis8vm1a6bid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1eqq827</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>How do people do their nails with shaky hands?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqq827/how_do_people_do_their_nails_with_shaky_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1eqpvml</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh look, a strawberry! 🍓 </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqpvml</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1eqpt3u</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Polish</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqpt3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1eqpmha</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Letting my nails grow: WEEK 10✨✨✨</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kntuqaquaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1eqpkrg</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l2juftduaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1eqp2b6</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>did my nails yesterday, what do you think? ✨🎀</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqp2b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1eqp03j</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails popping off?! </t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqp03j</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1eqovgf</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Textured press ons?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqovgf/textured_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1eqov2w</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>viva, brasil !!!!</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqov2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1eqoptf</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I Went Shorter Instead of My Normal Daggers</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp2t05p8oaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1eqoovr</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>First time playing around with Aurora Glass Paper!</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g42ii5o1oaid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1eqon5d</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Sour gummy nails!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfb2d5jmnaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1eqoell</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Lines/ripples in my nails</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqoell</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1eqo9fs</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>what is better gel x or acrylic?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqo9fs/what_is_better_gel_x_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1eqo6ab</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stiletto, soft gel </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egohwmadkaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1eqntww</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Evil Eye New Nail Day! 🧿</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqntww</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1eqns8s</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>One hand down, should I do the other?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqe7vaynhaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1eqnqz5</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Milky white and cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcensrzehaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1eqnln4</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Not sure what to ask for</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqnln4/not_sure_what_to_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1eqnipv</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>i usually get almond but i decided to switch it up this time. does this shape suit me at all or should i go back to almond next time?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqnipv</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1eqnex7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐾 I love how these turned out! 💅 </t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqnex7</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1eqnbgx</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP - MEGA X </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqnbgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1eqmsl9</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Sea set 🐚🪸🦭🌊🐋</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqmsl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1eqlw1d</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>new celestial set ✨💫</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9ts6r2f4aid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1eqlec6</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>My newest short set</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqlec6</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1eql0g1</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found these at Walmart from paintlab and thought they'd be perfect for my birthday tomorrow </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0594lsacy9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1eqky4y</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqky4y/beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1eqkta5</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>I’ve been obsessed with chrome lately</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arh18gixw9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1eqkl7r</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Nail Shaping tips?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqkl7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1eqkf9u</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black flash glitter French </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqkf9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1eqk83q</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>This design but all the possible colours I’ve done</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqk83q</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1eqhjrg</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Pearly Green &amp; Pink Floral Ocean theme (gel x by me)</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqhjrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1eqj462</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done professionally </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqj462</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1epv8h0</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Damaged nails from gel- will it grow back normal?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epv8h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1eqdsjn</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help :) </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqdsjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1eqeigv</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Salon wear</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqeigv/salon_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1eqgd6r</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Finally tried square :)</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu6szht329id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1eqgq3l</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure transformation </t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqgq3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1eqf9om</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqf9om</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1eqf7zi</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Gothic Barbie 🩷🔗</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3cdtzq2u8id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1eqex7m</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Simple nails at home</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek67pqcvr8id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1eqes3f</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I am not a huge fan of pink but I love how these turned out 🩷</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs4okrdvq8id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1eqcvp7</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>cat eye waves!</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh5crc4ec8id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1eqcsu8</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Regrowth help</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i69wqgdrb8id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1eqcffd</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqcffd</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1eqblez</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Just had to share my latest nail art</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y504sza118id1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1eqbkt1</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Gel x, hard gel, or poly?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eqbkt1/gel_x_hard_gel_or_poly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1eqayws</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Summer nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okynr0dbv7id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1eqywiz</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Stained nails?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqywiz/stained_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1eqyuv1</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Recommendation: Sky blue linear holo polishes?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqyuv1/recommendation_sky_blue_linear_holo_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1eqysua</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Why isn’t UNT available on Amazon?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqysua/why_isnt_unt_available_on_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1eqyr38</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Acrylate allergy question - stickers marketed as adhesive for press on nails safe?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqyr38/acrylate_allergy_question_stickers_marketed_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1eqyob6</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Any tips for swimmers?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqyob6/any_tips_for_swimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1eqxrvi</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I have the original OPI Nail Envy or no? </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqxrvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1eqxpun</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The nails and the inspo (her name is Sparkle) </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqxpun</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1eqxb97</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ORLY Terra Nova vs. ORLY Wild Natured </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqxb97</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1eqwz5g</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Utterly and absurdly pretty </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rfx70fiygcid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1eqwxbp</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle Remover </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqwxbp/cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1eqvxhl</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Best cremes?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqvxhl/best_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1eqvgi8</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mani I did for my upcoming trip to Louisiana </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqvgi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1equudm</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stained glass nails </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1equudm</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1eqtisd</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Really wishing I got a back up bottle of this 🥲</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqtisd</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1eqtd0u</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI - My Private Jet </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dwacaqsmbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1eqt8wz</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Pahlish - Lantsov Emerald</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1057zrjvlbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1eqsgw2</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>French sour apple rings</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqsgw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1eqrzp4</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Glass Stars Oops!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqrzp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1eqruyd</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Floss Gloss Dimepiece dupe?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqruyd/floss_gloss_dimepiece_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1eqqx6t</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>was quite impressed with this one - Sally Hansen Scram! 💚</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqqx6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1eqqqdu</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Feed Me!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqqqdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1eqprrb</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Emily de Molly haul!!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqprrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1eqp2pe</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">genuinely got a compliment with these nails! </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xss3tlftqaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1eqort7</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Found an ancient bottle of NFU  Oh 51!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiajagjmoaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1eqlgjg</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Nails very damaged from improper acrylics removal - are press ons a good temp solution?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqlgjg/nails_very_damaged_from_improper_acrylics_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1eqofhl</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Help! Has anyone had this happen with Mermaid Bait? What did I do?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqofhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1eqnyef</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Essie - "Second hand, first love" 010</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsrem1ddhaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1eqnego</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Cirque Colors soleil</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqnego</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1eqnc16</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>ILNP - MEGA X</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqnc16</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1eqnbii</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Jelly Skittle </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drpg7s1heaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1eqmz0w</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Winnesy thoughts?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r89cjgd0caid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1eqmoe9</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>LynB does it again!</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqmoe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1eqmnhy</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Leaf Peeping - What Addiction?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqmnhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1eqlyaa</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>White, milky drugstore or Ulta polish that doesn’t streak</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqlyaa/white_milky_drugstore_or_ulta_polish_that_doesnt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1eqlc97</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>10 free brands?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqlc97/10_free_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1eqlaww</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Swatched all my pretties and now I’m gonna sit on them like a dragon</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfxx1r5d0aid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1eqkq90</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Olive skittle - my first post here!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqkq90</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1eqk9he</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>The scream I scrumpt! (Blueprint, ILNP)</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvmcxo95t9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1eqjeca</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Blueprint or Bikini Bottoms from ILNP?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqjeca/blueprint_or_bikini_bottoms_from_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1eqiw8j</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Lynbdesigns</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eqiw8j/lynbdesigns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1eqiu4k</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Cirque x Jarritos 🫧</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C-kwssxOawe/?igsh=a3B3bjFzYXY0a2xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1eqihqd</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Zombie Claw PPU</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqihqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1eqi7n9</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Please help me match this colour!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0299llp3f9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1eqhstz</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Very ... slowly ... getting better... at stamping</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqhstz</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1eqfq7c</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>🌵Cacktooses🌵</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqfq7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1eqeuh9</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some nail polish pigments, for example magnetic and thermal, quickly explained on this video! </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://youtu.be/_rklMjEtrn4?si=t2y8N0b2EpSUv2sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1eqdxaw</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Possible Dupe</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqdxaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1eqdiv2</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Moonicorn-unicorn</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqdiv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1eqc20a</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Sigh.</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yozrbt4g58id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1eqbh8z</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying thermals and loving them! </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqbh8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1eq5v84</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Good nudes for pale olive complexion?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eq5v84/good_nudes_for_pale_olive_complexion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1eq9r9t</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eq9r9t/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1eq8tf6</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Advice for nail perfectionism</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eq8tf6/advice_for_nail_perfectionism/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1eqytz9</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax9xsfndycid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1eqxcji</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Comment your favorite set❤️😝</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqxcji</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1eqwcd3</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Fancy Shmancy!!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqwcd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1eqvf6g</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Road trip to Louisiana nails. </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jfl9xsh3cid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1equ7k9</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Ocean Inspired Nail Set</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55fnz8xitbid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1eqpy7s</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Las Vegas themed press on set I made for a nail model client, loved how this turned out! All hand painted by me</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmgprzz2xaid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1eqp5nm</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Moo-la-la</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqp5nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1eql44t</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colorful and shimmery </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eql44t</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1eqkudn</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sailor moon nails </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nspj5vc5x9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1eqkiac</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Black flash glitter French</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eqkiac</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1eqhl81</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>I keep my left hand nails short because I play guitar! credit to Ellen at O Nail Spa</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yg8v2elma9id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1eqfuva</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>First tutorial what do we think?🤗</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h4m13alky8id1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1eq9vve</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>i like them so much!!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pkgkc9qj7id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1eq9n5n</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Nail by @streetnail.art</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o30qjc1h7id1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1eq95dv</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eq95dv/help/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug 14 08:09:34 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C469"/>
+  <dimension ref="A1:C627"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8406,6 +8406,2692 @@
         </is>
       </c>
     </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1erw10c</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to get a hang on 3d flowers! </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6iiwo4o7lid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1eru3me</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>From grubs I was scared to photograph to talons ready to pierce the cube...what color should I paint them?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eru3me/from_grubs_i_was_scared_to_photograph_to_talons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ertv7m</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>i love my nail tech</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ertv7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ertan0</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Natural extensions</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckmmq1dxbkid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1erswn7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting dip powder at the salon. Are the edges supposed to look like this? </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erswn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1erskjn</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Picked up a new thermal polish 😍</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ws2oofsf4kid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1erqikn</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Black or White?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erqikn</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1erri6k</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>I adore cat eye polishes 🤩</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/75jv5ro6ujid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1errhq6</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>I adore cat eye polishes 🤩</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vhkkfmg2ujid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1errdyc</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Natural nail dip</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t3bd3x3tjid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1err4c1</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>What do we think ?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1err4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1erqw67</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>New to nails and wondering what to start with</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erqw67/new_to_nails_and_wondering_what_to_start_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1erqtws</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>for those who prefer press-ons..</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erqtws/for_those_who_prefer_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1erqnn1</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Love it or hate it !</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypmp68hrmjid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1erqi2v</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>First time making press ons, I think I did good w/ the actual nail designs but the nail shaping/sizing seems off</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erqi2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1erqfgf</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Correcting egg shell nails?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erqfgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1erp9qq</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Back to School!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erp9qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1erqcz5</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">made these today </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uvmvo88kjid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1erq841</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>By me 🩷</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erq841</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1erq6ij</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Blue lightning nail art I did for a concert!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zrc3lwnijid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1erp9xg</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Current press-ons :)</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecoko1bwajid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1erp30d</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>is there any kinda nail i can EASILY pop on an of? Just got a job that doesn’t allow nail polish and i love having my nails painted!!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erp30d/is_there_any_kinda_nail_i_can_easily_pop_on_an_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1erp15g</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Im-pressed by Chillhouse press-ons</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erp15g</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1erovk8</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Early August press-on nails orders that I made</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erovk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1erooop</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Going back to regular polish after using gel and I’m having a hard time </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erooop/going_back_to_regular_polish_after_using_gel_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1eroisj</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>I can no longer afford to keep up with my UV gel manicures right now. Any recommendations on how to remove them without completely destroying my real nails underneath?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eroisj/i_can_no_longer_afford_to_keep_up_with_my_uv_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ernqbz</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>how do i stop my polish from being soft and becoming messed up + sticking to fabric and fluff</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ernqbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ero6lm</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>please girl! ten cents good advice</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ero6lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ernz6a</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d64tiz40jid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ernsgh</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>What do u think?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e87tjhdmyiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ernlu5</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f36bsy25xiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ernl5k</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>1st builder gel mani, can I file?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odzoyeozwiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ern15p</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When your nails look like the galaxy </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm0h6t6jsiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1erhwyl</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Post-hard gel removal…what now?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erhwyl/posthard_gel_removalwhat_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1ermux6</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hand-painted blueberry nails! 🫐 </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84x1mmx4riid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1erlrog</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I love this chrome soo much</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffdvb9triiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1erlppt</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first home gel set! Beetles tips &amp; polish. </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v190vquciiid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1erlg5f</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sailor moon nails </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng6z93fegiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1erl4cw</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>What supplies do I need to DIY my nails? (Luminary)</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erl4cw/what_supplies_do_i_need_to_diy_my_nails_luminary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1erkt2f</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>When I tell my manicurist, "I'm going on a classy date"</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aporfsapbiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1erkhev</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Basic but never dull hahaha</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gadv1dr69iid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1erk6cj</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Cat 🐱 nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9lwcwm17iid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1erjjsv</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Getting in my bright summer manis while I can!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4glv3mte2iid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1eriqzr</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>First time trying chrome!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eriqzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1eri4nl</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Nails by my bestie</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w2hc2umphid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1erhy7n</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>My nails before vacation. How would you rate them? 1-10</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erhy7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1erh9t6</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">is it obvious these are press ons? </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erh9t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1erh86m</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>At Home Nail Techs - Houston</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erh86m/at_home_nail_techs_houston/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1erh69b</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Long natural nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqwlhhhtihid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1erg4vy</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Repair Help </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erg4vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1erh10m</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Birthday set 🥳🎉💞</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rbo445shhid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ergn82</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Question from a guy who doesn't get his nails done often:</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdkx2emxehid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1erg6ur</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly press ons! </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljnyw55pbhid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1erbimk</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Press on removal?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d3s5u8begid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1erff7y</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guess which one is gel x! </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoz9zme26hid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1erfxbh</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>are my nails long enough for coffin nails?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn4txokq9hid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1erfhn8</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>milky lavender (?) what do we think??</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erfhn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1er0u36</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Tried Chrome Nails at Home using Regular Polish &amp; Powder from I Love My Polish</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bclljgirkdid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1er5m0f</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>This design reminds me of a country's flag but I can't remember which one! 🤔</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8i6eiqg4fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1er747c</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>New Nails!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er747c</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1er79um</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er79um</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1er7ic3</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel so powerful with these nails </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er7ic3</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1erej1e</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Recently did this 90's inspired set. Guess who!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erej1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1erf82w</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape or length is best for my hands? </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erf82w</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1erdvvi</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Beach vacation press ons!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erdvvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1erf3jd</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Cowgirl galactic 👽🐮</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erf3jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1erevov</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>My new nails🎉</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk8mpjya2hid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1erejbf</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Do you like this design?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/816z6vytzgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1eredp2</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This months set.. I looove them. </t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmxfptfoygid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1er2qls</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Eyeshadow trick</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er2qls</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ere9qa</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long or short </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ere9qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1ere7xz</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Which color looks better on my hands?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c60u523jxgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ere57y</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Thank you everyone for your opinions. 😊 I went with Oval shape. Bonus pictures for everyone who was worried about my ring finger 😂</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ere57y</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1erdtg2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Does oil based nail polish remover work on dip?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erdtg2/does_oil_based_nail_polish_remover_work_on_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ercpdl</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Wedding nails for a new client!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhbpzlpomgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ercfe4</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Just sharing my misery</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ercfe4</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1erc9ax</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>What would you rate them from 1-10?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfuz685hjgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1erbx5b</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Posting old sets: freestyle Halloween </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erbx5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1erbujg</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Avocat Nails 😻</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2l1o0nvlggid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1erbms4</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Acrylic brushes are EXPENSIVE!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erbms4/acrylic_brushes_are_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1erbing</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Bartending/Nailcissisr</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1erbing/bartendingnailcissisr/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1eramof</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Want to recreate this with gel polish and chrome powder</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke6snxu18gid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1eralvb</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Getting fiber gel? today, need some advice</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eralvb/getting_fiber_gel_today_need_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1eraawr</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>What are your favorite nail gel brands?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eraawr/what_are_your_favorite_nail_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1era8uk</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What styles would suit me? </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1era8uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1er98zn</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Butterfly 🦋 Nails</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er98zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1er81kc</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ordered $5 on- sale imperfect nails from Static </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1er81kc/ordered_5_on_sale_imperfect_nails_from_static/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1er81c1</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel retention better than Polygel? </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1er81c1/builder_gel_retention_better_than_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1er7i40</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>What brand of gel base &amp; top coat do you use?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kxpm3avkfid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1er7i3f</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails due for an infill? </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er7i3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1er5w4y</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>My first time getting acrylic nails (25€) any opinions/Advice?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze8192t17fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1er5s5n</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>What an eyesore…</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14crhsh16fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1er5muq</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>The square style never goes out of fashion! But for me they are so uncomfortable</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e5vg8co4fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1er5lcn</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>loving this shade of wine red 🍷</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gc9dura4fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1er5law</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>First attempt at Polygel</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q83wlh694fid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1er4le6</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>so proud of this set!!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er4le6</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ervby1</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After a few bad nail appointments, it's back to doing it myself :) </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ervby1</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1eruvc3</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>LynB Designs "Name That Prune"</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eruvc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1eru72s</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>cirque should do a hi chew collab next</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eru72s/cirque_should_do_a_hi_chew_collab_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ertlvx</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Orchid jelly sandwich ✨👾</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ertlvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ersnzv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Cirque Colors Eros Jelly 😈🍇💜</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br1av0ld5kid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ersg9o</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Blocked by indie polish brand?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ersg9o/blocked_by_indie_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1errlps</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just darling 🎀⛲️🦢 would u wear? </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1errlps</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1erraa7</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings of Fire 🔥</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erraa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1erqglm</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Don’t Touch the Calico Bush! - Krisable Designs / PPU rewind 24’</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erqglm</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1erq46u</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings!! AHHHH !!!😍😍</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erq46u</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1erpm36</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Looking for 1980s nail polish still made today!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erpm36/looking_for_1980s_nail_polish_still_made_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1erooi4</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>yay or nay? essie tropic low</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erooi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ercymn</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Exploring Death Valley </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vi1cy17jogid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1erng8z</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Any transparent magnet polishes?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erng8z/any_transparent_magnet_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ern4wq</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Foot fetish</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ern4wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ern18s</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>First time painting on fake nails separately first instead of on my hands!</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgomeyrjsiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1erm3cn</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>🥹 The wishlist is organized</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/477e08o6liid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1erlg8w</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>easy and sweet cat lady nails 😻</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr7ken3fgiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1erl5i5</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Shake Your Shamrock 🍀</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h51lqu8eiid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1erikyw</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I Think it Smells Like…</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erikyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1eriae8</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Very ... slowly ... learning ... stamping</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eriae8</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1erhm7l</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>help with regular lacquer and chrome/eyeshadow</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erhm7l/help_with_regular_lacquer_and_chromeeyeshadow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1erh1oz</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Dupe request:  pale yellow</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erh1oz/dupe_request_pale_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ergprt</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>First time doing gel at home (OPI Malaga Wine)</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ergprt</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1erey1c</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Combined my polish collection with my mother's collection. </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgtsn8br2hid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ere6dn</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>KBShimmer "Flip Out"</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb53c504xgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1erdpba</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can’t open bottle?! </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erdpba/cant_open_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1erdgos</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Cheetah print for summer</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib0nn5d5sgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1erdb4p</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Tips for keeping nails nice in medical field?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erdb4p/tips_for_keeping_nails_nice_in_medical_field/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1erd3ve</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Some questions from a Newbie</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erd3ve/some_questions_from_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ercg8g</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Seche Vive or Sally H Insta-Dri?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ercg8g/seche_vive_or_sally_h_instadri/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1erbyjm</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Shimmery purple night sky nails</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mklwk41dhgid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1erbwob</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velveteen Rabbit 🐇 </t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erbwob</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1erbbmj</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Crystal Knockout-25 fly</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erbbmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1erajhx</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Customer service rant</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1erajhx/customer_service_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1er8vv8</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Extra sparkle for my maternity shoot </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wd7czfdkvfid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1er8dit</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Why does salon polish take so long to dry??</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1er8dit/why_does_salon_polish_take_so_long_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1er7vsq</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Beginner help! Gel polish making my nails thin?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1er7vsq/beginner_help_gel_polish_making_my_nails_thin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1er7rvt</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>[Looking for recommendations] Would someone share a nail polish that resembles this lilac sparkle?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1er7rvt/looking_for_recommendations_would_someone_share_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1er6zci</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this shade more than I thought I would! </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er6zci</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1er4mkx</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Abstract velvet art with Mooncat</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er4mkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1er3tto</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>To backup or not to backup 🤔</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1er3tto/to_backup_or_not_to_backup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1er2wzs</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>I didn't get any work done today and I blame it all on Lorraine</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1er2wzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1eru429</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>New to the sub, and wanted to share some designs I’ve gotten!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eru429</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ertr5i</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Did some hand painted Mario kart nails🎮🏎️</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkyxke2xgkid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1erricp</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Neon colors ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zwimo98ujid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1errgk3</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>I adore cat eye polishes 🤩</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qiypz6nrtjid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1errgme</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Blue and green💙💚 lo</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4nwytgstjid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1errdi7</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>One of my favorite designs ?/10💜🩵💛</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlkgvj6zsjid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1erqlp8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>First time making press ons, I think I did good w/ the actual nail designs but the nail shaping/sizing seems off</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erqlp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1erpjps</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not a professional, but would like to be, any tips? </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erpjps</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1erob9q</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Fluted Glass Nail Trend</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erob9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ermwr6</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time painting on fake nails instead of my own hands! 🫐 </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1crm7sjriid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ermiga</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>The best of the week. I only practise extension with SoftGel. What do you think of this tecnic? Hace any advice?🤍</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ermiga</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1erjqc2</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>New design 🖤</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yj35xlmr3iid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1erifnb</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hacker Movie Nail Set 💅 </t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erifnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1erh0km</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>What do you think of this Carey effect? The only thing I thought when doing this work for my client was: I NEED TO DO IT ON ALL MY NAILS NOW🤣</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erh0km</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ergina</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Boyfriend picked my nail design 🏁</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ergina</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1erduo4</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>i think i outdid myself 🧏🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erduo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1erb7fr</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Nails love ♡</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tep0xdw2cgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1erb1zt</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Probably ten steps away from selling these </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23fsgy21bgid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1eravzk</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>I love you! You?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh1tnmlv9gid1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug 15 08:09:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C627"/>
+  <dimension ref="A1:C798"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11092,6 +11092,2913 @@
         </is>
       </c>
     </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1esohdq</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Was $25 a fair price for these?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54dj09p0yrid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1esnm3w</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>been practicing russian manicures+gel application for the past couple months</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/267q3puvnrid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1esn9n3</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new set </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhwb0it2krid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1esn8wp</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Aura nails (pressies)</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esn8wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1esn6fo</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Strawberry moon nails 🍓🌙</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6zbj6z2jrid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1esmx46</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>my euro summer nails !! 🌞</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1irg20c9grid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1esmmfd</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Guy tries a marble nail</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esmmfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1esm2kd</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>gel-x french tip 🤍</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1sggz3d7rid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1eslzqr</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Princess nails🥰</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afbh8irk6rid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1esl26d</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Back to school 😁</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boyfkrbpxqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1esl08n</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Newbie question about hard gel</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmggz8q7xqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1eskryg</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>I’m almost 30 years old and this is my first time ever getting a full acrylic set! What do you think? :)</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eskryg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1esk4v2</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd and 4th pics are my faves </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esk4v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1esk38g</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little gems 💎 </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/taku0gb0pqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1esjk7v</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjjppzhmkqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1esiopg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>I adore cat eye polishes 🤩</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4oxrve86dqid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1esiomm</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>I finally finished my Deadpool &amp; Wolverine nail set! Hope you like the special feature 🥰🙌</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lsti2d56dqid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1esi4i3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Hyper realistic French manicure</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esi4i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1eshe5l</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nakies! No time for a full mani, but I needed to clean them up a bit. Oil, oil, oil! </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eshe5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1eshbdr</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Did I exaggerate a little? I love appliqués</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tqlj5il1qid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1esh99k</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first set of custom pressons! </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esh99k</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1esh7j3</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Just got a shipment and couldn’t help myself</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esh7j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1esgc4t</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>press ons anybody?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esgc4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1esg76s</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Press on removal</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esg76s/press_on_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1esfw0t</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>New Fill</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrt52c2gqpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1esfspg</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Muppet nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esfspg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1esfrlk</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I cut my cuticles for the first time, how did I do; any pointers?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esfrlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1esfq2p</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Taste the rainbow</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esfq2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1esfoda</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Nail tech accused me of slander?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esfoda/nail_tech_accused_me_of_slander/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1esfl2s</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>black sets always look so clean🖤</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q75hly71opid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1esfje5</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>I swear they're cuter irl</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs4de1bonpid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1esfh9j</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>I love the color 😍</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t30ua578npid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1es60an</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>idkk</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es60an</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1esdk0t</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Less Streaky dupe of Sally Hansen Nail Rehab? </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqlmm8qj8pid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1esan3v</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I go back? </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esan3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1esc1l1</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>E-file damage</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esc1l1/efile_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1esd0ge</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>How do I remove nail glue from a press on nail?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esd0ge/how_do_i_remove_nail_glue_from_a_press_on_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1escz0r</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first full set </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1escz0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1esc4sz</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Need suggestions</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esc4sz/need_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1esb64j</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Saw a redditor use the overcast collection from ilnp, I never made an order to so fast, not as well done as the og but I absoulutly adore em😍</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esb64j</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1esb2b7</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>DND Mermaid Glitter is the GOAT</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzjnm3kbqoid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1esb068</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First order. What do you think? </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsnoqxbwpoid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1esamxd</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blink182 nails. Me and hubby's matching nails at the end </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cdddxupvmoid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1esaltg</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>obsessed with these &lt;3</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esaltg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1esajn4</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My new nails I did!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgdrgnhzloid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1esa22v</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A super delicate design </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gdh7ewkhoid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1es9l48</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv9v8fy4eoid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1es9c43</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>rate my at home nails!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es9c43</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1es95no</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Sally Hansen’s Hooked on Onyx &amp; Glitter Glam Manicure.</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d34j2cozaoid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1es93m4</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunset vibes </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es93m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1es8dib</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>When should I get my nails filled?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es8dib</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1es8lqz</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Does gel x cut off my nails?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxxr0rlz6oid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1es7nh1</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Bio gel manicure keeps lifting as a full sheet from natural nail. Nail tech/application problem or is it just my nails?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es7nh1/bio_gel_manicure_keeps_lifting_as_a_full_sheet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1erxqii</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Can I get these shortened? How short?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqegq6o9slid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1erouz8</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madam Glam order was stolen </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erouz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1es8d6b</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Feeling spooky do I did these on myself</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es8d6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1es8b63</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Is it weird if I bring my own gel nail polish to salon?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es8b63/is_it_weird_if_i_bring_my_own_gel_nail_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1es84qp</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Plain overlay?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es84qp/plain_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1es82g7</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oggw42063oid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1es7z8s</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what’s the best method/products for securing nail charms on lacquer? </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es7z8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1es7umh</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Second try on almond nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es7umh</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1es7nm9</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Lustrous Lightning 🌩️</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es7nm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1es7cwn</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This set was done at Nailux Spalon in Woodbury. Truly stunning!! </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr03qb02ynid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1es6xz5</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lime green to end off the summer :) </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hdtmxn3vnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1es6usl</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new croc nails! </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es6usl</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ery2dg</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I put builder gel on over filed thin nails? </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ery2dg/can_i_put_builder_gel_on_over_filed_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1es5ov7</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Gel polish discoloration?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ituz7405mnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1es1wzw</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Surreal and wonderful experience yesterday </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es1wzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1es1cwu</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What to ask for at nail salon to strengthen my natural nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es1cwu/what_to_ask_for_at_nail_salon_to_strengthen_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1es6kfc</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>MY POLYGEL NAIL IS FINALLY STAYING ON!!!!!!! AFTER A YEAR OF DOING NAILS</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpq9nzaesnid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1es6k6u</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>my bf learnt to do nails only for me!! 🥹</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unpgpkncsnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1es6aiu</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>🐸</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es6aiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1es62dx</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fave nail design I did on my nails so far! Do you guys like it too? </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9j8vvwtonid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1es2hu3</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Would you pay 3 chocolate coins and one cookie for these nails?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es2hu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1es5bdx</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Is rubbing alcohol allowed in checked baggage??</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es5bdx/is_rubbing_alcohol_allowed_in_checked_baggage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1es5b9b</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye is not cat eyeing </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es5b9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1es4zy7</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>blue nails for today</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejg49xl9hnid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1es4hko</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Flower nails for summer -Maybe the first and last before autumn season</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es4hko</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1es4bhn</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>My Go To Dreamy Set ✨</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es4bhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1es425m</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my natural nails are the longest they’ve ever been! </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es425m</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1es3y4p</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Woof</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ywb65n2anid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1es3sti</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>My nails this past 4th of July</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es3sti</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1es3qtr</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Sunset-Beachy Vibes♥️🥰</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7y7kfkp8nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1es3pm0</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Evil Eye Toe Nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfxp5egg8nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1es3oko</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Practicing my nail art:)</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vogg6jw88nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1es3ly7</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Toes</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es3ly7/toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1es3f67</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Evil Eye Flower Nails 🧿💙🪬</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z7gqvyc6nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1es3ecb</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple Mini French </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47gubv076nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1es2uqj</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I have to improve my technic 🥲</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv27uymb2nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1es2mhd</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know these are plain but I LOVE this color </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y49bw9gn0nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1es187d</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>My Toesies</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apynqljvpmid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1es0rw0</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>In love with this set! 😍</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es0rw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1es0q6e</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>DIY gel mani</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1es0q6e/diy_gel_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1es0h1h</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Pink Zebra Nails! 🩷🦓✨️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es0h1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1eryjzi</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>i did my nails the other day, opinions?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr7pb6691mid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1erxhof</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Idea for my next set</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s85ziu8fplid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1erwsh0</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I’ve been craving a fun set for so long!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5pr3p01hlid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1erwkqf</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Obsessed with nail stickers</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erwkqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1espd3e</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Ex Nail Biter</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1espd3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1esob9z</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>I'm in love with "Am I Everything You Fear?"</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esob9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1esncp1</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Obsessed with nail stickers</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esncp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1eslnmc</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>ILNP ink one coat</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gatfmue3rid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1esl21d</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Any brand recs for collab?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esl21d/any_brand_recs_for_collab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1eskkcy</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Can you help me find the most beautiful magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eskkcy/can_you_help_me_find_the_most_beautiful_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1esjtp7</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Layering experiment!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esjtp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1esjmzm</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>🐛🍎Apples🍎🐛</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esjmzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1esirux</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Is Lucky Jelly (Cirque Colors) a good dupe for Cherry Jelly (Lights Lacquer)? If not, any suggestions?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5xqxcoxdqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1esinge</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Chemical X </t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esinge</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1esifw4</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Freshly done so ignore my dry cuticles lol</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esifw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1eshvv5</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>To me it is Fall now 🥹</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x67pdkj6qid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1eshkre</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Wanting to buy OPI Gel polish, but I’m not a “pro”. Help?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eshkre/wanting_to_buy_opi_gel_polish_but_im_not_a_pro/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1esh9rs</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first set of custom pressons! </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esh99k</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1esggmz</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Update: A color to match this Lego piece</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m1jh7s0vpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1esfo7u</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Shades that are similar to the pink in this poster? Saw this concert last night, and they used this color a lot in the show, and now I want to find a polish to match</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0ipd8ehopid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1esfeac</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learning how to do my nails at home </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceiirx0nmpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1esfait</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know a shade that would come close to this one? Thank you!!! </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sarck1gtlpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1esf7sc</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautometry inaccurate pre order estimates? </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esf7sc/beautometry_inaccurate_pre_order_estimates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1esei2h</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Dupe for Holo Taco Cold Slate?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7hoojeqfpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1esef59</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Now Go And Don't Look Back</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esef59</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1esea77</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Pop Arazzi polish</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esea77</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1esdu4l</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Fast drying, DIY manicure tips for new mom.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esdu4l/fast_drying_diy_manicure_tips_for_new_mom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1esdkv8</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It certainly glows </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwxoadrr8pid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1escs4e</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Silhouette + Subtle Spider </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1escs4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1eschx9</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>list of indie Halloween Advents</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eschx9/list_of_indie_halloween_advents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1escevw</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>It's giving highlighter, pumpkin candy pail, orange tic tac...</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzvngsk40pid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1esalj2</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time wearing a thermal polish, and I am mesmerized! </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esalj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1es9yit</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Gradient thing :)</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es9yit</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1es96ta</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been loving Sour Note from Holo Taco </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnc89iz7boid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1es8jft</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Water marbling and a flower</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es8jft</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1es7qhw</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Party nails for my husband's bday</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es7qhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1es7l10</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Lustrous Lightning 🌩️</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es7l10</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1es6n8m</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>New nail shape, who dis?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htocyi6xsnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1es6dhy</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>When your nails inadvertently match your knitting project 😍</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es6cnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1es6d99</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco Deeply Superficial </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4gy4fzzqnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1es5cqo</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Solace</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es5cqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1es510t</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>best top coat for magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1es510t/best_top_coat_for_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1es4ao1</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She ripped off my nails and b**** one in the process </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1es4ao1/she_ripped_off_my_nails_and_b_one_in_the_process/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1es3wdd</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Question about descriptions</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1es3wdd/question_about_descriptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1es3e7u</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>LynBDesigns haul and mani (first order)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es3e7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1es1o9d</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Surreal and wonderful experience yesterday </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es1o9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1es1bdq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>UD Asphyxia update! (Combo manicure)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifd7luxlqmid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1es0b9t</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally put on Shake Your Shamrock ☘️ </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es0b9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1erz70x</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My dr strange inspired nail art</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv9bthtt7mid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1ery7f7</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Dupe Request for Cirques Flaminglow</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ery7f7</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1ery4kz</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Vibrant colours for the last few weeks of Summer 🪸 🧡</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st8uodwkwlid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1esoepr</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Struggling with 3d characters </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esoepr</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1esoeg1</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sneak peak at press on set hand painted </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rowrqkq0xrid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1esnfx3</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>first attempt at doing nails</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxunwyg0mrid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1esmxpf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>I wanted to try an exotic design and this came out</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98nvsusfgrid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1eskana</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>My set for Splash House this past weekend</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uukznn9rqqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1esk3jq</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>What do you think of yellow?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs90pws2pqid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1esjr7t</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Just trying to support my aunties nail art/youtube journey…. https://youtube.com/@nails-by-vitilougo?si=ZJBOGRXm3q1p2oEi</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1esjr7t/just_trying_to_support_my_aunties_nail_artyoutube/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1esip2c</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>I finally finished my Deadpool &amp; Wolverine nail set! Hope you like the special feature 🥰🙌</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/27o97qz9dqid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1eshl1r</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>App or 3D models for designing nails?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eshl1r/app_or_3d_models_for_designing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1eshcjd</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my new nails </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1zvt6s22qid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1esgdgj</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Circus set ! This took forever to sculpt😅</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hot40mobupid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1esf456</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>cute lil blueberry nails (ik the bow charm may not completelyy go with the set but I got them yesterday and got excited lol)</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bez6vb9fkpid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1esardb</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with blooming gel </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esardb</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1es8tbv</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpdikaji8oid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1es7ggu</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>This set was done at Nailux Spalon in Woodbury. So gorg 💅✨</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32i09ahsynid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1es548b</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legend of mana nails </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es548b</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1es4gi7</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Love this design</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bswft4vhdnid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1es4eli</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sanrio Nails! </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es4eli</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1es42hr</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Eyeball Nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23j9pqeuanid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1es41hf</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Nail my girlfriend did :)</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1es41hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1es40yy</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Evil Eye Flower Nails</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9izbvwokanid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1es3zvx</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Evil Eye Toe Nails🧿💙🪬</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9rcuyudanid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1es3mmj</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Practicing my nail art:)</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5q10zsv7nid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1erzkdk</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>What would you call this?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2axfoagbmid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1erwtel</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>What is the best (AFFORDABLE) 3d sculpting gel?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1erwtel</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1erwhrj</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>So adorable and kawaii 🥰 💅🏼</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5rvp65cdlid1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug 16 08:10:12 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C798"/>
+  <dimension ref="A1:C967"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13999,6 +13999,2879 @@
         </is>
       </c>
     </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1etiufx</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>did this set on myself earlier! theme was fairy core lol 🧚🏼‍♂️✨</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlv0c48wczid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1etihrt</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Abstract nails</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etihrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1etibct</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Working on some extra pressons 💕</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etibct</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1ethzem</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Black chrome, french tippies 💞</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ethzem</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ethyfu</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Does anyone else really like short stiletto nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i11t36e32zid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1etguz9</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching nails! </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etguz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1etgc96</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Can I buff off the top coat?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c1bek0njyid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1etfy23</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>todays gel x set :)</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlt6chocfyid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1etfxbp</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leopard print frenchies I did on myself 🥰🥰 I’ll post a better pic tomorrow </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi3pgfw4fyid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1etfvpp</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Do these look busted or what?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etfvpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1etfskz</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done dk how to feel </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4eg4z1sdyid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1etdcd9</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Growing out salon damage so going with press ons for now. Wow?? Impressed by imPress!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kk5d1uvlqxid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1etd9je</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>New set. Electric Blue &amp; Pink Chrome with 3D designs.</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etd9je</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1et2yez</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>how do i fix this?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r8wzgw3ivid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1et3u67</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nail too far into nail bed? </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et3u67/press_on_nail_too_far_into_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1etcyiy</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>What are some good but cheap brushes for nail art?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etcyiy/what_are_some_good_but_cheap_brushes_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1etdwx8</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>How do you get along with matte effect nails? they struggle a lot</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hadhbegsvxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1etfgze</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Clear dip and then gel ?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7soxw0kkayid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1etenxo</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>DIY set, I think these turned out kind of pretty</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etenxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1etel1u</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Stir the pot</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etel1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1etejec</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail broke </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etejec</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1eteg8t</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>This</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v96a8q8q0yid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1etdq7r</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer flowers 💐 </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etdq7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1etdoww</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Beginner nails</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etdoww</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1etd2cn</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this a good shape? </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etd2cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1et4u9a</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Canadian Nail Schools?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq62lbtavvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1et5sdd</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Nail shape and stress biting</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et5sdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1etcnpo</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>French mani with Hello Kitty nail stickers on my natural nails ❤️🎀🌷</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etcnpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1etc96p</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Flames and more flames. Done at Fingerbang in Portland, OR</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2ghcixzgxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1etbvth</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0p0g47tdxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1etbpep</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st Try @ Tequila nails ! </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etbpep</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1et516d</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>How do I get these darn stars to not peel up?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czwndweqwvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1et6dom</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>First acrylics and I hate them</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1wax7wj6wid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1et6fhh</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Scooby Doo!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et6fhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1et6yzc</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">any package handlers here? </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et6yzc/any_package_handlers_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1et57mt</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Tips on making sticky tabs work?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et57mt/tips_on_making_sticky_tabs_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1etbh1t</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>New set. 🧡🩵💜💙</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etbh1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1etb13d</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Where can I buy OPI gel polishes online?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etb13d/where_can_i_buy_opi_gel_polishes_online/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1etaj0y</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love!🐞What do you think? </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mijn0ili2xid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1etafs3</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I gave myself such a neat manicure, tell me honestly, what do you think?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhux30hl1xid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1eta6hj</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Getting our nails done always brightens our days! what is your favorite tone?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yakzvapizwid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1eta5cl</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Nail techs talking trash about other salons</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eta5cl/nail_techs_talking_trash_about_other_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1et9sqd</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sun and moon 🌙 </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9sqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1et9rmc</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>my nail tech is the best (first time posting)</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9rmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1et9chv</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>I love these!!!!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9chv</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1et9avr</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Freshly done yesterday...</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8n80arlswid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1et9ajh</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Is a shellac “fill” a thing?..</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et9ajh/is_a_shellac_fill_a_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1et8x2j</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Do you like chrome ?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y2d3bujpwid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1et8sqf</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>🦋 🌈</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8cwgn8lowid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1et8440</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Press-ons I did as practice!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et8440</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1et7o5x</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pedicure </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2thgps11gwid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1et71wj</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Recommendations for nail techs in Atlanta???</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et71wj/recommendations_for_nail_techs_in_atlanta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1et6ru4</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Loving this color "Kiss my Aries" by OPI. Simple yet beautiful.</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lae8j17f9wid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1et6med</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink sparkle frenchies💖 </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yu4morb8wid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1et61qo</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>How to clean up sides?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3aq4azz44wid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1et5z7h</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>New set. Not sure how I feel about them.</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et5z7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1et5jli</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GelX Press Ons </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et5jli/gelx_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1et5i7a</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape will suit my hands? </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et5i7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1et55tm</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails after a long depressive episode. I can’t tell if I hate it </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4k5vqcnxvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1et4ma7</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Glowing summer set</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et4ma7</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1et4llb</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’ve been doing nails for around 8 months.. started to have this problem from the start i’ve tried to paint the gel thinner or even priming under the gel polish but nothing has worked.. after a week my polish peels/chips off </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl81b4b0tvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1et4ftm</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>brat nails 💚</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et4ftm</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1et4do9</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et4do9</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1et41tq</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Groovy tortoise shell nails 🐢🌼</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et41tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1et3jro</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Need help / recommendations!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g90mvgj2mvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1et3i9r</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Halloween set already! Lol</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyablylslvid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1et3asp</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>idk what to call these but i love them!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et3asp</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1et2wc8</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do you like my new set? </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv547iqphvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1et2cum</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>How can I get started in nail art?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1et2cum/how_can_i_get_started_in_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1et2cr6</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Cloud nails ☁️💕</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et2cr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1et1z2s</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>how I love doing my nails</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30fdaxi8bvid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1et1fcd</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple but cute!! </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et1fcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1et19md</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Three months ago I started doing nails and this is my result today... what do you think?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxdzfe346vid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1et16dl</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>What do u think? Too classic? 🤍</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hymxun7g5vid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1et0rge</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>How do these look?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3h8cx4h2vid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1et0cia</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>A fresh set makes everything feel a little better</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et0cia</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1et0bb5</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>First time getting encapsulated nails!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et0bb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1et08mm</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">still having a hard time with straight consistent lines tips welcome </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwffknonyuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1et05l6</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of these 3D nails, with rhinestones and beautiful details... I love them? </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5thytp3yuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1eszyu6</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>new set on natural nails💎</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eszyu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1eszt0v</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Shorties to close out Summer</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7z3ykrjvuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1eszshs</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>so in love with these floral nails! 💐</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plarx6zfvuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1eszggt</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>How about this ink style?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4dghrazsuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1eszgc3</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my nails properly done for the first time (gel on natural nails) </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eszgc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1esyum0</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arizona tea </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2ykjlikouid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1esymqu</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Weird thumb aside, I got my nails done and they're SO PRETTY</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo66o0iymuid1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1esy8yy</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>imPRESSed with imPRESS!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh842ox6kuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1esnn4m</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seashell Inspired for Summer 🐚 </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esnn4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1esr0kk</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Press on nails - Can I put glue on my nail first, and then the sticky tab next?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esr0kk/press_on_nails_can_i_put_glue_on_my_nail_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1esjld6</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what am i doing wrong with the jello jello pell off base ? </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esjld6/what_am_i_doing_wrong_with_the_jello_jello_pell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1est8sh</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>What if Disney knows people are selling nails featuring their characters? Other brands also apply.</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1est8sh/what_if_disney_knows_people_are_selling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1esx0h1</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Any tips for a newbie to clean up my cuticles?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf8ehnhdbuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1eswdry</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>1st time doing polygel nails with paper forms!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eswdry</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1esvlnt</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>My press-ons for the week</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esvlnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1esvgmd</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>First time doing gel nail extensions!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1esvgmd/first_time_doing_gel_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1esvbrk</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I woke up this morning and my nail had broken. </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp2kpy6xytid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1esvavw</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>my first attempt at doing my nails at home, how did i do?🙂</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtj71m7qytid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1esuo72</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Where’s the beach?!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esuo72</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1esunop</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>This set is called “ I wish I had a pool” lol</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esunop</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1esukps</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought you guys would like this sheer nude cat eye </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vmjp9pxxstid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1etirjk</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Who has an I Scream Nails - Opal Obsession swatch for me?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etirjk/who_has_an_i_scream_nails_opal_obsession_swatch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ethvc8</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Electric eel vibes ONLY ⚡️</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/slt0kbv01zid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ethu6i</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Sassy Sauce "Wet Spot" from July '24 PPU</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ethu6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ethblj</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Can I just say this subreddit is absolutely amazing</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ethblj/can_i_just_say_this_subreddit_is_absolutely/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1etgmsd</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Mini Lurid Haul Review</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etgmsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1etfohz</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Testing/comparing SJ 3Designs velvet magnets!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etfohz</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1etfk8h</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>throwback to my brat nails from july</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etfk8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1etet5o</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>will my polishes go bad in the heat?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etet5o/will_my_polishes_go_bad_in_the_heat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1etenp1</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Why is my nail polish not sticking here?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9mrmico2yid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1eteje6</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Stir the pot</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eteje6</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1etdnfs</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>You, of Unshakable Conviction</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5r0aiewdtxid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1etdk9m</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Meh-light</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etdk9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1etczv0</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LynB layered skittle </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dul3vnpinxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1etcxuw</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else get lucky with BKL Crabs Is Bugs? </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c041ndvzmxid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1etchpm</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>When the tipwear gets bad, but the polish is too pretty to remove</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etchpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1etbpi6</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>what polishes do you recommend for the "my nails but better" look?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v23v737acxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1etb8q0</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Chihiro by Ethereal</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytl1zh2e8xid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1etap5l</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>House Of Hades</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etap5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1etahye</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco Amber Apathy </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etahye</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1et9qo0</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Sparkli</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9qo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1et9pw7</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Two DVN shades :)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9pw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1et9n5y</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>BKL mystery and polish sneak peaks?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et9n5y/bkl_mystery_and_polish_sneak_peaks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1et9m3u</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Come Again by Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17hneiv1vwid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1et9jku</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I'm super disappointed by the Cirque x Jarritos collab. Five plain jellies nearly identical to shades they were already selling, and a plain holo glitter topper?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mywdg0miuwid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1et92zq</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Back to shorties (kinda)</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et92zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1et8qrq</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Cirque Haul</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2zydct6owid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1et7xxy</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>What’s a nail polish innovation you’d like to see? (like new texture, formula, color)</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et7xxy/whats_a_nail_polish_innovation_youd_like_to_see/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1et7u7e</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Self leveling polish! </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et7u7e/self_leveling_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1et60zi</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Outlined French Tips</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et60zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1et4dy1</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Skyrim polishes? </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et4dy1/bkl_skyrim_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1et4adh</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Concert Nails Featuring My Cat 🐱💚</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et4adh</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1et31p1</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal Layering </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et31p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1et29m9</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Pick a color for me!!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et29m9/pick_a_color_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1et22l3</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>LynB Designs Zoisite - my new favorite nail polish</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et22l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1et1lk8</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>lazy rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et1lk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1et1j3n</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>2nd Attempt at Chrome</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et1j3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1et1g1v</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Removing laquer painted over gel base</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1et1g1v/removing_laquer_painted_over_gel_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1eszre4</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Attempted a "gray"dient chrome!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eszre4</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1eszm41</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>I know they’re still short but this is the longest I’ve ever been able to grow my nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8wwkb06uuid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1esz019</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Zippers. F**king zippers man.</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esz019/zippers_fking_zippers_man/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1esyzkt</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Cirque x Jarritos collab</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esyzkt/cirque_x_jarritos_collab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1esye44</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Would appreciate suggestions on which of these might be best for cool olive skin?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esye44/would_appreciate_suggestions_on_which_of_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1esy8wm</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Gel Polish Recommendations?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esy8wm/gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1esxkkv</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Growing nails</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esxkkv/growing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1esvtub</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layering Experiment </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cn3qq8fr2uid1</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1esve4a</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Blushing Queens</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esve4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1esuwkq</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnetic tips and matching jelly in my favorite colors. I’ve peaked. </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esuwkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1esu7s2</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Kate bishop (Hawkeye) inspired nail art</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfinqnowptid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1esu6ii</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Can't believe I waited so long to wear this!? (Ethereal Lacquer - She likes my spark)</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esu6ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1esrz8g</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail care advice needed - looking for how to fix my husband's nails </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whbgz8xf4tid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1esqdq9</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Polish color changing over time?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1esqdq9/polish_color_changing_over_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1eth7i5</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Tried a new technique!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eth7i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1etg0e0</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>This design gives me space vibes, for the stars</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuys1nu0gyid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1etfb33</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>love when my clients ask me for rabbits on their nails🐰</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etfb33</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ete0km</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I did for VPC a Ceto Company </t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9votepnpwxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ete0j4</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Did you use these nails when they were in trend? what do you think?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bknnz6pwxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1etdqzr</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer flowers 💐 </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etdqzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1etdfzm</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leopard nails </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etdfzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1etdaat</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Flames and more flames! Done at Fingerbang in Portland, OR</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arcn7ip2qxid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1etai4e</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>We decided to experiment, please tell me how you like it?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf573sk72xid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1etahax</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Character Nail Art</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etahax</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1et9tcb</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sun and moon 🌙 </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et9tcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1et6izu</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>My Nails 💖</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et6izu</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1et4h76</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Glowing hot summer set</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et4h76</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1et465e</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Groovy tortoise shell nails 🐢🌼</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et465e</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1et2qq6</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Birthday nails hand painted on myself 💅🏼💫</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1et2qq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1esutqi</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>This set is called “I wish I had a pool” lol</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1esutqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1est00a</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>What do you think about my new work? I’m in love ❤️</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1est00a</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1esrzi3</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>How did they do?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pso3kd2j4tid1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug 17 08:08:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C967"/>
+  <dimension ref="A1:C1122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16872,6 +16872,2641 @@
         </is>
       </c>
     </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1eubxte</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mismatch for the win 🙂‍↕️ </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rgxeui4vd6jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1eubher</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>BIAB/builder gel and tips for long extensions?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eubher/biabbuilder_gel_and_tips_for_long_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1eubbab</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Sometimes I like bright pink</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkl5p9fu56jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1euan19</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>blue and white combination for today</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq35d5cfy5jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1euabav</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Super funky pink nails</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvcdrl1su5jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1eua8b8</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>I think grey is my favourite colour from now on!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ybx5a4vt5jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1eua1l4</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nails! 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eua1l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1eu8vzu</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Fill timing advice?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu8vzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1eu8mrh</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Put on press-on nails for the first time in a long time, what are these faded areas?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu8mrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1eu7o41</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink nail polish = lifestyle ✨️ 💕 </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0rtu1lw35jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1eu6zym</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Basic but always sparkling</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ijcq0dlpx4jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1eu6una</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>nails i did on myself today :3</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oci3uildw4jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1eu6tng</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Love this color💖</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu6tng</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1eu6o98</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday nails! </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3aqdqrfru4jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1eu6mta</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new nails 💘 my girl always hits it out of the park! </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu6mta</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1eu67it</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>First time doing my own acrylics.</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu67it</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1eu5y4t</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Lemon Nails or amalfi coast nails?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu5y4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1eu5nzm</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Purple Fire 😈🔥</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqx555cql4jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1eu54o1</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>See through pastel colors?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eu54o1/see_through_pastel_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1eu3bml</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>please help this nails newbie! ❤️</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu3bml</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1eu4tis</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutesy </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu4tis</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1eu4hsc</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutesy </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu4hsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1eu4a38</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>new coral pink set</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu4a38</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1eu3pyv</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying red nails. I think I love it </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6id75nl54jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1eu3bqy</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>🥹🥹🥹</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlrvrh3d24jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1eu30sn</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is this nail trend called? Photo by @nailbayo on IG </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksdeuriyz3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1eu31c4</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>My favorite I’ve done to date!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu31c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1eu2ymv</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have tried gel over natural and all kind of extensions, and only press ons are getting my fidelity </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu2ymv</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1eu2ku5</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>questions about custom press ons, and also some questions about nail art in general!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eu2ku5/questions_about_custom_press_ons_and_also_some/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1eu24g9</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Did my own gel nails</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu24g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1eu1x1j</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Has anyone tried the press-on nail brand “Nailcissist”?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxubsr79r3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1eu1kqr</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Conflicted on how these turned out :/</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jkq9pwko3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1eu0iax</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Favourite milky pink/nude recommendations please?? (Found on @bhambnails‘s page on insta)</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/broagd5lg3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1eu0x5r</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Hello im new here, i gotten some fake nail tips like 2 -3 weeks ago and im wondering do i need a fill or a new set?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsmq97zlj3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1eu0x21</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Did I pay too much?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1116ei2lj3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1eu0ko2</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>What do you think of my new nail design?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu0ko2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1eu0b2f</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Smell</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eu0b2f/smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1eu05t0</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time using gel </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqauxxayd3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1etzri4</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Iowa State Fair Nails!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etzri4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1etz5am</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel polish on skin </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etz5am</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1etyu9e</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally got this effect </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbtdbfkx33jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1etyny6</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>best nail shape for short fingers?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ddhoi6i23jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1etynre</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Learning to get a steady hand with the sticker placement but still very happy with these 🩷🎀</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kx7s1tm23jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1etyhlx</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>🦓!!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etyhlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1etyfmt</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last years  Halloween set </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etyfmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1etxt3a</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Tried something new with my nail polish</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etxt3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1etxk8b</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Be honest: these are bad right?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etxk8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1etxif4</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>TJMaxx win</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oi4klttt2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1etx8qt</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Pink Coffin Set 🩷</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etx8qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1etwz1f</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>I really enjoyed making this design</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex046amvp2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1etwbsz</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>This might be my favorite set ever</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etwbsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1etwb7c</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green before the summer leaves </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ckj66dwk2jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1etw8gh</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>This took me so long</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyq42eock2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ethe71</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome Love </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ethe71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1etmj3m</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>First try at dip went well! Buuut I didnt think about the shape/color combo...</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etmj3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1etqr89</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>So depressing.. How do you guys stop this from happening?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnps0hi4h1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1etvhke</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Low break on natural nail and extension, can’t decide what to do</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ujcwv6ue2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1etw3dj</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Asked for coffin, definitely didn't get that, but I think they're still pretty!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etw3dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1etvlw5</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Vintage and floral! I love doing my nails</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z989g0wof2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1etvjgu</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>August set ❤️💅</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbrwkeg8f2jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1etvak3</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie with builder gel </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynl2yhedd2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1etuwlx</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gray- warm nude cateye (russian mani!) </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etuwlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1etuhm1</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I did for a EVP of VPC a Ceto Company to wear for a conference </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb7pzqam72jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ettrnw</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>first time trying milky nails🤍</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ettrnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1ett7av</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>I have my dream natural nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88ymiyuey1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1etswn4</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber nail suggestions </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etswn4/rubber_nail_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1etso6d</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v85x4dyhu1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ets9hj</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylics and pedicure </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ets9hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ets5yh</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Magenta Candy</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwatyfb1r1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1etrz8b</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>1 year acrylic free!! clean af 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adirokvop1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1etqyw3</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching nails! </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyk141imi1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1etqufc</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I lost count of how many “engagement” manis I’ve done, but I’m so happy this was THE set 🤭</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etqufc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1etqqya</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Whimsical Cotton Candy Mermaid Vibes? 🩷🩵</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a84g4i32h1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1etqa6h</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Purple on purple on purple</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfvqjhvqd1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1etq0m1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Shorter for the first time</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etq0m1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1etpui7</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time with this shape and 4 years since last acrylic </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etpui7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1etp60j</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Update, I got my nails done!</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etp60j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1etp1d4</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel extensions! </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etp1d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1etp0an</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My nails need to be beautified</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/850j61fb41jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1etokpb</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>When the nails match the book just right…</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etokpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1etoek6</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Gel X Nails as Press Ons?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etoek6/gel_x_nails_as_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1etocfm</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cyberpunk dragonfly nails, glow in dark </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m8wzlx23z0jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1etnzyb</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>First post here!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bptgi5ew0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1etmxri</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>What do you think of my new design? Yes or not ?👍🏻👎🏻</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlqylkecn0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1etmuhl</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>longer lasting polish?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etmuhl/longer_lasting_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1etmnzj</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>CND VINYLUX “Untitled Bronze” Long Wear Polish Manicure</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvep2reyk0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1etm5nm</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Pettylicious 🐆</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etm5nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1etm3w9</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>acrylic nail questions</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1etm3w9/acrylic_nail_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1etllmc</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Nail tech ruined my nails, I hate them. More info in comments</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ulambcba0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1etlbtd</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">summer snow cone nails 🍧 </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08r5bb5870jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1etl0ge</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etl0ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1etjnpp</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Nude chrome</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etjnpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1etjh6j</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Former nail biter :)</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etjh6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1etjfk7</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Ethereal nails</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etjfk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1eucf4d</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>RIP to my brat summer nails 😭</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eucf4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1euaaly</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Rainbow Velvet 🧲</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/97f2r9weu5jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1eu92oh</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Crushed Holo</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu92oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1eu7zyi</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Painting over greenies - yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eu7zyi/painting_over_greenies_yay_or_nay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1eu7hya</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Starrily’s Nectar possible Encryption Key Dupe?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eu7hya/starrilys_nectar_possible_encryption_key_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1eu7364</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Shake Your Shamrock w/ Butterfly Effect</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu7364</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1eu5o6g</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dollar tree polish! </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu5o6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1eu45w8</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>So I just painted my nails yesterday so I'm not gonna change it but my first ILNP polish arrived!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5on8eq594jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1eu44cr</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squishy DIY magnetic </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bp5jbn8q84jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1eu2wz4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Swatched my collection</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zig1r65z3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1eu2u43</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Glass Dragons 🐉</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu2u43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1eu2ky5</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Does neon *always* fade?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8iowyw2kw3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1eu22x5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>LynB Designs - I Did a Punch!</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4c7y82ks3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1eu1umz</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Looking for alternatives for thorough body exfoliation tools/accessories that are long nail friendly</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctvtnomiq3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1eu0fak</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>gray- warm nude cateye (russian mani!)</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eu0fak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1etzrmw</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>creamsicle</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0jo9yq0b3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1etz7o9</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Help me create a Gel Polish SDS master-sheet?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>/r/GelNails/comments/1etz6br/help_me_create_a_gel_polish_sds_mastersheet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1etz6u5</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Advice for removing yellow staining on nails?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etz6u5/advice_for_removing_yellow_staining_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1etyw9r</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>ISO the best fancy purple polish!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etyw9r/iso_the_best_fancy_purple_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1etyt9t</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Lemon’s coming back! 🍋✨🪩</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7vldqg1q33jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1etyo22</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Favourite sheer polishes for layering and creating different looks?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etyo22/favourite_sheer_polishes_for_layering_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1etyiit</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>show me your favorite shiny sheer shimmers! your glass frog-likes! your ether dragon types!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etyiit/show_me_your_favorite_shiny_sheer_shimmers_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1etya79</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Swipe to see the magic ✨️</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etya79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ety5tg</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Whatttt 🤯</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q7jwfgwoy2jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1etxs7x</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>cirque colors citron jelly</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etxs7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1etxdjx</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Mid Level Shear - Stella Chroma</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1im8qp1qs2jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1etxawz</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Pink Coffin Set 🩷</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etxawz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1etx947</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">date night nails! paired with black heels and hot pink sunglasses </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o25q4y2wr2jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1etwsyj</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>missing hawai’i!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etwsyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1etwr15</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Full Scream Ahead 🤝 Wedgie </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etwr15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1etwobk</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Starter Kit: What should I buy?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj5mqd4mn2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1etw731</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flowerchild </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv16npd2k2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1eturtf</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Sharing my skittle I made using the Peanut Butter &amp; Holo Jelly bundle.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eturtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1etuhji</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Might need sunglasses for this one 😎</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etuhji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1etu6c8</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to doing my own acrylics, and am struggling with nail tip fit. </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etu6c8/new_to_doing_my_own_acrylics_and_am_struggling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1etu428</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>ILNP - Cygnus Loop (love that shifty shift!)</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77vnnu9u42jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1etts7y</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s my undertone? Help with proposal nails!! </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pky52d4j22jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ettkdg</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Farm Rio Inspo</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ettkdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ett976</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Submitted by dissertation for review and am celebrating having free time again with a neon gradient (PR) </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ett976</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ets7rj</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An update on the green polish I'm looking for. </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ets7rj/an_update_on_the_green_polish_im_looking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1etr2vw</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>House of Hades - Mooncat</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etr2vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1etqeyu</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Bottles for mixing your own</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1etqeyu/bottles_for_mixing_your_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1etp1xx</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>BKL medley (I can never just stick to one)</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etp1xx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1etoyd2</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Black pearl nails?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rlqndfx31jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1eto2ra</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>⚡️💚Green Ranger💚⚡️</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eto2ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1etnfxw</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Jade nails</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etnfxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1etmzhb</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>advice for press on pricing</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etmzhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1etme2n</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>greens most similar to this?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etme2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1etm72h</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Pettylicious 🐆</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etm72h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1etluw3</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Cheri Cheri Lady 🍒</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zm7n41zyc0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1etejus</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Kept getting distracted while sewing today!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4aw90fo1yid1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1eu7hmt</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Mermaid style art nail made by me</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7xt2ax025jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1eu23ra</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do y’all plan your nail sets? </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtgt5xqqs3jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1etz5vx</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Quick Totoro inspired set i threw together to wear to a a party this weekend!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lramnz2c63jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1etxdv2</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips on what to improve? </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow00tkovs2jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ets4i7</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>MATTE NAILS WITH SOME MARBLE😍😍</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfalk0vqq1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1etqlka</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Saga for the Perfect Pink Part 3</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in0vm9u1g1jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1etqetu</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nails done by myself </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etqetu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1etoe8l</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cyberpunk dragonfly nails | glow in dark gel used </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/meorn7lhz0jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1etmst5</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>3rd set attempt from yesterday</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai0toap5m0jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1etm443</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Repost of my cute nail art</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1etm443</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug 18 08:08:36 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_18.xlsx
+++ b/data/2024_08_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1122"/>
+  <dimension ref="A1:C1297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19507,6 +19507,2981 @@
         </is>
       </c>
     </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ev3v0z</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nail advice?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ev3v0z/nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ev3mll</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Thoughts…m48 first timer</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2piaqk2ykdjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ev3j1c</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Wanted some colour for summer✨</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy5b11vojdjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ev3j04</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Chrome 🍬</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iff8uwwojdjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ev2vep</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galaxy $7 press on nails: one week later </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7aiwbyjbdjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ev24wa</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Lilac french tips</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00h37ud03djd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ev1agj</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>My new blue nails! 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5j1x3hqtcjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ev0z3s</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Airbrushed nail design ✨💕</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngshb0f8qcjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ev0v2f</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape suits me better? </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ev0v2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ev0q80</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hmu8ex0kncjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1euzzt3</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Press Ons I made for my day-after-birthday dinner with my parents</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euzzt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1euzt6p</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfp3ijr4ecjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1euyzrt</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Nails !! Cute?? </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dru5isiz5cjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1euyy65</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been growing my nails for a while and they’ve all been breaking off slowly 😭 </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zalo4rjj5cjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1euyaqu</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzkz3zq5zbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1euxug2</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>What do you think? metallic silver</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6cuyd5tubjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1euxj86</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did my nails! First time with glue on </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dackjvourbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1eux95t</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Hello Kitty press ons 🥰</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj1egsyapbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1euwrn3</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails! </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v3cvc7zkbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1euwktc</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Honey Bee press ons I did as practice!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euwktc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1euvv7s</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euvv7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1euvsex</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euvsex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1euvrrz</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>she’s a star 🌟</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euvrrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1euvb82</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>I feel like they’re… missing something 🤌🏿🤌🏿….</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euvb82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1euv94v</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>When you feel bad about yourself…</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1euv94v/when_you_feel_bad_about_yourself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1euv3sz</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Help pls!?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1ifly6a6bjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1euuks3</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>anyway to take acrylics off at home??</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1euuks3/anyway_to_take_acrylics_off_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1euuich</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Questions about surgery?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64uvpa4c1bjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1euuc8z</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>At home gel nails</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkdqqkqwzajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1euteqo</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Corporate goth </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iy0tlpccsajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1eut9m4</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Found my new fave</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyhbwqe7rajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1eut9lc</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last summery nails before labor day! </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eut9lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1eut63m</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Beach Party Nails</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwd4juehqajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1euszou</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Chrome + Pearls</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b29wmwb0pajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1euswqu</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>the force is strong in this one</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euswqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1eusvqs</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly Bean nails </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusvqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1eus8f8</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">looking for a deeper (?) nude </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eus8f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1eusnam</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Royal Flush</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusnam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1eusleu</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Color changing nail polish had me wishing it was winter already!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusleu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1eusg4d</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">before &amp; after (+reference) </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusg4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1eusawe</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Newest set ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rot9vxejajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1eus2g0</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>First time with almond.</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj0ok91jhajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1eudyv8</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need Help with Nail Shape and Style – Feeling Unsatisfied with My Natural Nails </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eudyv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1eudzc7</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Happiness is long painted natural nails 💅 M(30) What would your reaction be seeing me in public ?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eudzc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1eugkb0</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Square or round?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eugkb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1euh8s2</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Reminder to give your nails a break :)</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euh8s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1eukbv1</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Pink Chrome Moment 💖</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izr9wqcrs8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1eun0w4</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>What I wanted vs what I got</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eun0w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1eung4u</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Golden bird - pedi sets serie #1</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eung4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1eupc8b</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>How do you like this color?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5e9vqlxv9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1euqwq3</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Bad first acrylic nails experience - how to salvage?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euqwq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1eurlpf</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Were these worth $65+tip?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eurlpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1euraww</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>It's fall, you can't tell me otherwise! 🎃🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euraww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1eurejz</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>In love with my new nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edq1qujfcajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1euref4</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>moth nails i wore to pride today! all done free hand including sculpting the moths :)</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euref4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1eur97f</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eur97f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1eur7mx</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newest set </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eur7mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1euqw61</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Summery tulip-style nails</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euqw61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1euq8x5</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Beach vacay nails are ready 😍🌊</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rddbmy873ajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1euq0bj</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>summer nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1euq0bj/summer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1eupx9k</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I copied all the stuff my salon uses and did them at home myself! Not bad!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9ucdxll0ajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1eupwvp</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grow nails for wedding in 1m or go fake? </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eupwvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1eupo1e</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Vacay nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqdtlzhiy9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1eupaok</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>New Shape</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eupaok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1euopvo</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I’ve done god knows how many designs on my nails, but a classic nude nail remains unmatched…</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqmpzts0r9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1euomee</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Very Demure. Very Mindful. 😉</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euomee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1euoa3f</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail shape is best suited for me? </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrmm4mfjn9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1euo747</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Give me all your stocky hands nail advice/recs</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euo747</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1eunx45</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Flower Nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eunx45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1eunrho</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Neon Superhighway</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crbjfzsgj9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1eunizp</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Regular polish..</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eunizp/regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1eunhee</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Itty bitty press on set</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bat7wiq7h9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1eunejp</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail shape is best for my nail beds? </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eunejp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1eun07w</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My boyfriend said they make him think of ice cream </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jbaioxgd9jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1eumnap</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Should you pay for a nail repair if it happened the same day?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eumnap/should_you_pay_for_a_nail_repair_if_it_happened/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1eumh43</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are these any good? </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eumh43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1eulgpq</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very cute </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cna17hsj19jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1eukwpl</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>what color is this nail polish ?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khhv5laax8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1euko9q</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">press on nails look very wide? is that normal? </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euko9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1eukhme</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Should I do commissions for my press ons?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eukhme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1eujtlr</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>This was my current manicurist's first job for me</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lf0g4q8m88jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1euivgu</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Question about pedicures and such</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1euivgu/question_about_pedicures_and_such/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1euilxl</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m loving this deep red for the upcoming fall months! </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8585aroye8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1euibdb</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Beginner nail art ideas ?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euibdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1eui5dx</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Space theme</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ob83l55b8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1euhnkk</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>How long do you think it would take for that butterfly to fly away?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ju1f3e078jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1euhckj</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Second attempt at doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/piofvavd48jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1eugvlg</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two left hands,  no problem </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3htlds408jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1eugok8</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>First time doing gel x</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjnrbrycy7jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1eug3l5</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Art nail on natural nails </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mw6s72us7jd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1eufqbu</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Pink nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cndaafd1p7jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1euf2qi</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some pokemon themed nails, the totodile evolution line </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euf2qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1euf14e</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Took me two hours and I think I failed (not my hands)</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7lgjw85h7jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1eueqyj</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tip advice </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eueqyj/french_tip_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1euef9n</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Orange glitter</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cmttppas97jd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1eueej1</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>milky white evil eye nails🧿🦢</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki2on1he97jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1eudqwn</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Bit shy but got asked about the full set so I wanted to share it!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/revf9xwd17jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1eudmwz</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>My summer nails (in Paris)</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwvvy45yz6jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ev2wvo</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>First ombre in 5 years. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ev2wvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ev2rm2</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>gel polish and regular polish</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ev2rm2/gel_polish_and_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ev1zm8</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ev1zm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ev14wb</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>I like to do nails when I'm sad. Here's the fresh manicure I gave my beautiful mama 💕</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh6j6kvzrcjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ev0qbk</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>What will be the most sought after polish in the future?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ev0qbk/what_will_be_the_most_sought_after_polish_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1euzkf1</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Never Sleep Again- Cuticula ❤️🖤🛌</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euzkf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1euzblq</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Always back to neutrals &lt;3</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euzblq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1euzbgt</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Favorite base and top coats?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euzbgt/favorite_base_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1euz59f</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>I love this beautiful decoration although it is already getting damaged.              I call this beautiful decoration Alegria, it inspires me with joy and peace every time I love it, I don't know, but it's beautiful.</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euz59f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1euz0nl</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>I love this beautiful decoration although it is already getting damaged</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euz0nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1euycg8</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>What have been your random sources of inspo for manis?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euycg8/what_have_been_your_random_sources_of_inspo_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1euxoag</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>ready for vampire szn 🩸</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd5m5ta6tbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1euwltf</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Anybody has both Mercury in retrograde (mooncat) and Skye (ILNP)?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euwltf/anybody_has_both_mercury_in_retrograde_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1euwj1v</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone ever tried using washi tape on their nails? </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euwj1v/has_anyone_ever_tried_using_washi_tape_on_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1euwbtd</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Order from cupcake polish came in✨</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iseq9xyygbjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1euw2sr</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>This is giving me poker night vibes</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20yyhqqpebjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1euviyz</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else match their manicure to the ceiling of their hotel lobby? </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euviyz/anyone_else_match_their_manicure_to_the_ceiling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1euvenu</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>My first time re-wearing a polish. Because I love it! My first thermal and one of the first indies I ever wore. LynB Design’s “Peony For Your Thoughts”</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mlnewjv8bjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1euv9id</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Atomic Sherbet by ILNP</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euv9id</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1euuyba</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>First more complicated(for me) look! A sunset gradient@</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euuyba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1euuv71</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Shorties</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c92wijk94bjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1euuqlx</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Little Chef - Cuticula</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euuqlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1euuo2u</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alien Infatuation </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euuo2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1euulba</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t know why I slept on Lurid Lacquer’s Indomitable for so long. </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euulba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1euu3wf</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Sheer Happiness </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euu3wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1eutnfb</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sour Apple Rings made me buy these brat boots </t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eutnfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1eutlcq</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>"Rainy Diamond Beach"</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs5bssvltajd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1eut50l</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIYed a jelly out of old cheap polishes I don't really like. I know what I have left of the bottle won't last because it's already getting clumpy (last pic) but it looks so juicy and the experiment was fun. No spider this time! </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eut50l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1eusq0g</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I give up on trying to do gel nails at home! 3rd time trying, and can’t seem to get them right. Going back to regular NP at home. What’s your favorite NP at the moment?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eusq0g/i_give_up_on_trying_to_do_gel_nails_at_home_3rd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1eusled</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Accidental 80s gradient</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82zun9lslajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1eusl7z</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta-Dry 'Powerslide'</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s66g5mirlajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1euraap</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First manicure I did myself- ILNP deep space . In love with this color! </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euraap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1euquns</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Feeling some Bottled Rage?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/go0e2p0x7ajd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1euqfif</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Cirque Colors Lyra - my first magnetic!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euqfif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1euqcjg</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Lorraine 💙</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euqcjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1eupzf3</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chanel Immortelle 135 Dupe? </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eupzf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1euoqmg</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>I just really need it to be autumn already</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euoqmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1euoml1</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polished for Days - Melt </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euoml1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1euoj53</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maelstrom by Mooncat </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euoj53</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1euoi60</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>O.C.W Blue Glitter by Cairuo</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/BHcVy8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1euog3a</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Is it necessary to use cuticle remover? HELP!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euog3a/is_it_necessary_to_use_cuticle_remover_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1euo3em</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Please tell me this is salvageable</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk04la22m9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1eunwx8</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I’ve been too indecisive lately to use the same polish on both hands 😍</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eunwx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1eunu1x</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Took the gels off for a break…</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eunu1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1eunjbp</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You know what, you DO need another shade of blue-green </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk0gb65nh9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1eunatj</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Vampy red for pale skin, timeless I'd say!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eunatj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1eumol5</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Meh meh meh all the way home </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjyt7w7wa9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1eumnsp</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I call this colour my "grandma polish" because it reminds me of the polishes my grandma used. Bunny helped me with the pics, don't swipe if you are scared of (cute) jumping spiders, I just have to show off my babies on every occasion </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eumnsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1euml47</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>I love Kyoto pearl opi for a clean look- work with my hands and it doesn’t chip</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9ok1i55a9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1eul5ey</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Sparkly French nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6q1f0l6z8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1euky5b</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>What was your gateway polish?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vidohzkx8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1eukjxc</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>ORLY x Lisa Frank</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnljk2fku8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1euk2ij</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail colors for platinum rings? </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euk2ij/nail_colors_for_platinum_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1eujion</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">budget friendly polish </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eujion</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1euj8t6</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Kamek-worthy polish?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4diu1nj4k8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1euitq3</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Atomic sour apple rings and narf</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj74p9cpg8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1euikur</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Subtle watermelon vibes 🍉</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euikur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1euifgi</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Does anyone else keep the little boxes?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euifgi/does_anyone_else_keep_the_little_boxes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1euhcpb</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Slush + Lovebird jelly sandwich </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euhcpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1eug834</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Watched Promising Young Woman for the first time - Loved the movie and her skittle manicure 💗🎀</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eug834</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1euel35</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Humidity and UV glue</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1euel35/humidity_and_uv_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1eudegu</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I right or lefthanded? </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eudegu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ev40wq</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate and suggestions! </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb2wxcv1qdjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1euzr62</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>I am just a beginner ..😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rrxusu3idcjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1euzauw</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tips plz!! </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euzauw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1euxz74</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set I made today, thoughts? </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euxz74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1euukph</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fave nail sets I have gotten so far!! </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1euukph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1eut1dl</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>What's the best gel polish brand for intricate, detailed nail art?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eut1dl/whats_the_best_gel_polish_brand_for_intricate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1eusq09</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusq09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1eusimw</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Tried some new polishes</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eusimw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1eusba9</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Newest set 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qq38l4ijajd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1euom7r</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Gold steel using? My client say yes🥵🥇</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1xda9t7q9jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1eun7p5</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Golden bird - pedi sets serie #1</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eun7p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1eul04u</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Can anyone help?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/865ebxv3y8jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1eukidh</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I do commissions for my press ons? </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eukidh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1euk5rs</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Clueless dad seeking advice</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1euk5rs/clueless_dad_seeking_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1eugi5h</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pinks!! </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmerg0rpw7jd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>